<commit_message>
Extend vertinimai file with other parts
</commit_message>
<xml_diff>
--- a/vertinimai.xlsx
+++ b/vertinimai.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justaskalpokas/PycharmProjects/eda_atsiskaitymas_2022_12_10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikassvazas/Desktop/codeacademy/eda_atsiskaitymas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B3D6FD-951D-4B4E-9CFB-ED5475F039AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A2ABA9-4F34-C44B-8056-E705029E4CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D8938A20-A77F-724E-A8A8-09A9297ED3D5}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D8938A20-A77F-724E-A8A8-09A9297ED3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Vardas</t>
-  </si>
-  <si>
-    <t>Pavarde</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>3 dalis</t>
   </si>
@@ -56,16 +50,49 @@
     <t>3 (max 0.5)</t>
   </si>
   <si>
-    <t>Dovilė</t>
-  </si>
-  <si>
-    <t>Dobravolskaitė</t>
-  </si>
-  <si>
-    <t>Irmantas</t>
-  </si>
-  <si>
-    <t>Kaunietis</t>
+    <t>1 dalis</t>
+  </si>
+  <si>
+    <t>2 dalis</t>
+  </si>
+  <si>
+    <t>Šarūnas Steckis</t>
+  </si>
+  <si>
+    <t>Darius Baronas</t>
+  </si>
+  <si>
+    <t>Dovilė Dobravolskaitė</t>
+  </si>
+  <si>
+    <t>Aistis Bagdonas</t>
+  </si>
+  <si>
+    <t>Vilius Stankevičius</t>
+  </si>
+  <si>
+    <t>Skirmantė Vaišnoraitė</t>
+  </si>
+  <si>
+    <t>Mantas Pieža</t>
+  </si>
+  <si>
+    <t>Tautvydas Raibikis</t>
+  </si>
+  <si>
+    <t>Irmantas Kaunietis</t>
+  </si>
+  <si>
+    <t>Mikas Šimoliūnas</t>
+  </si>
+  <si>
+    <t>Julius Henrikas Barauskas</t>
+  </si>
+  <si>
+    <t>Studentas</t>
+  </si>
+  <si>
+    <t>Viso</t>
   </si>
   <si>
     <t>0.5</t>
@@ -75,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,16 +110,110 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF434343"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,14 +221,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,125 +584,616 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE4723D-84D6-F941-B2B9-02C19B8B649C}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="18" width="13.1640625" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D1" t="s">
+    <row r="1" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="E2" s="4">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4">
+        <v>6</v>
+      </c>
+      <c r="I2" s="4">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4">
+        <v>11</v>
+      </c>
+      <c r="N2" s="4">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4">
+        <v>13</v>
+      </c>
+      <c r="P2" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4">
+        <v>16</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="9"/>
+    </row>
+    <row r="4" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="9"/>
+    </row>
+    <row r="5" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="8">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="T5" s="8">
+        <v>0</v>
+      </c>
+      <c r="U5" s="8">
+        <v>0</v>
+      </c>
+      <c r="V5" s="9"/>
+    </row>
+    <row r="6" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" s="8">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="U11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="9"/>
+    </row>
+    <row r="14" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+    </row>
+    <row r="17" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+    </row>
+    <row r="19" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+    </row>
+    <row r="20" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K27" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:R1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="29" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>